<commit_message>
oops I broke the keynote
</commit_message>
<xml_diff>
--- a/lang stims concatenated.xlsx
+++ b/lang stims concatenated.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="20080" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="0" windowWidth="21980" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>George Square</t>
-  </si>
-  <si>
-    <t>Chris Triangle</t>
-  </si>
-  <si>
-    <t>Robin Star</t>
-  </si>
-  <si>
-    <t>Mel Heart</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>bounc</t>
   </si>
@@ -46,6 +34,60 @@
   </si>
   <si>
     <t>stopp</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>AgentName</t>
+  </si>
+  <si>
+    <t>AgentShape</t>
+  </si>
+  <si>
+    <t>PatientName</t>
+  </si>
+  <si>
+    <t>PatientShape</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>ProgressiveSentence</t>
+  </si>
+  <si>
+    <t>VerbStem</t>
+  </si>
+  <si>
+    <t>Verb</t>
+  </si>
+  <si>
+    <t>PastSentence</t>
+  </si>
+  <si>
+    <t>ShapeProgressiveSentence</t>
+  </si>
+  <si>
+    <t>ShapePastSentence</t>
   </si>
 </sst>
 </file>
@@ -77,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -126,14 +174,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -149,6 +211,11 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -164,6 +231,11 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,114 +565,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f>CONCATENATE($A2, " ", $B2, " is ",$E2, "ing ",$C2, " ", $D2,".")</f>
+        <v>Kyle Square is stopping Lily Triangle.</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>CONCATENATE("The ", $B2, " is ",$E2, "ing ","the ", $D2,".")</f>
+        <v>The Square is stopping the Triangle.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G8" si="0">CONCATENATE($A3, " ", $B3, " is ",E3, "ing ",C3, " ", D3,".")</f>
+        <v>Lily Triangle is bouncing Zach Star.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="str">
-        <f>CONCATENATE(A1," is ",B1, "ing ",A2,".")</f>
-        <v>George Square is stopping Chris Triangle.</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Zach Star is rolling Melissa Heart.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  is shaking  .</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  is balancing  .</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  is ing  .</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  is ing  .</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="G9" t="str">
+        <f>CONCATENATE(B4," is ",E2, "ing ",D4,".")</f>
+        <v>Star is stopping Heart.</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="G10" t="str">
+        <f>CONCATENATE(D4," is ",E2, "ing ",B2,".")</f>
+        <v>Heart is stopping Square.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="G11" t="str">
+        <f>CONCATENATE(D4," is ",E2, "ing ",B3,".")</f>
+        <v>Heart is stopping Triangle.</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="G12" t="str">
+        <f>CONCATENATE(D4," is ",E2, "ing ",B4,".")</f>
+        <v>Heart is stopping Star.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f>A13+2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B17" si="1">A14+2</f>
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f>CONCATENATE(A1," is ",B1, "ing ",A3,".")</f>
-        <v>George Square is stopping Robin Star.</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C3" t="str">
-        <f>CONCATENATE(A1," is ",B1, "ing ",A4,".")</f>
-        <v>George Square is stopping Mel Heart.</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C4" t="str">
-        <f>CONCATENATE(A2," is ",B1, "ing ",A1,".")</f>
-        <v>Chris Triangle is stopping George Square.</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C5" t="str">
-        <f>CONCATENATE(A2," is ",B1, "ing ",A3,".")</f>
-        <v>Chris Triangle is stopping Robin Star.</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="C6" t="str">
-        <f>CONCATENATE(A3," is ",B1, "ing ",A1,".")</f>
-        <v>Robin Star is stopping George Square.</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="C7" t="str">
-        <f>CONCATENATE(A3," is ",B1, "ing ",A2,".")</f>
-        <v>Robin Star is stopping Chris Triangle.</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" t="str">
-        <f>CONCATENATE(A3," is ",B1, "ing ",A4,".")</f>
-        <v>Robin Star is stopping Mel Heart.</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" t="str">
-        <f>CONCATENATE(A4," is ",B1, "ing ",A1,".")</f>
-        <v>Mel Heart is stopping George Square.</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="C10" t="str">
-        <f>CONCATENATE(A4," is ",B1, "ing ",A2,".")</f>
-        <v>Mel Heart is stopping Chris Triangle.</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="C11" t="str">
-        <f>CONCATENATE(A4," is ",B1, "ing ",A3,".")</f>
-        <v>Mel Heart is stopping Robin Star.</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finished concatenated lang sims table
</commit_message>
<xml_diff>
--- a/lang stims concatenated.xlsx
+++ b/lang stims concatenated.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26230"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilyjordan/Desktop/EvLab/GitHub stuff/AgentPatientStimuli/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="21980" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="10560" yWindow="460" windowWidth="21980" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>bounc</t>
   </si>
@@ -88,6 +93,18 @@
   </si>
   <si>
     <t>ShapePastSentence</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>bounce</t>
+  </si>
+  <si>
+    <t>shake</t>
+  </si>
+  <si>
+    <t>balance</t>
   </si>
 </sst>
 </file>
@@ -240,6 +257,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -567,11 +589,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.33203125" customWidth="1"/>
@@ -579,7 +601,7 @@
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -611,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -626,6 +648,9 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="str">
         <f>CONCATENATE($A2, " ", $B2, " is ",$E2, "ing ",$C2, " ", $D2,".")</f>
@@ -636,7 +661,7 @@
         <v>The Square is stopping the Triangle.</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -651,13 +676,16 @@
       </c>
       <c r="E3" t="s">
         <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G8" si="0">CONCATENATE($A3, " ", $B3, " is ",E3, "ing ",C3, " ", D3,".")</f>
         <v>Lily Triangle is bouncing Zach Star.</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -671,6 +699,9 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="str">
@@ -678,61 +709,67 @@
         <v>Zach Star is rolling Melissa Heart.</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  is shaking  .</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  is balancing  .</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G7" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  is ing  .</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G8" s="1" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  is ing  .</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G9" t="str">
         <f>CONCATENATE(B4," is ",E2, "ing ",D4,".")</f>
         <v>Star is stopping Heart.</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G10" t="str">
         <f>CONCATENATE(D4," is ",E2, "ing ",B2,".")</f>
         <v>Heart is stopping Square.</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G11" t="str">
         <f>CONCATENATE(D4," is ",E2, "ing ",B3,".")</f>
         <v>Heart is stopping Triangle.</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G12" t="str">
         <f>CONCATENATE(D4," is ",E2, "ing ",B4,".")</f>
         <v>Heart is stopping Star.</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -741,7 +778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -750,7 +787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -760,7 +797,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -769,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5</v>
       </c>
@@ -781,10 +818,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>